<commit_message>
Updated version and installers
updated the installers to be the current version of the app.
</commit_message>
<xml_diff>
--- a/ChorelistGenerator_Output/ChoreList.xlsx
+++ b/ChorelistGenerator_Output/ChoreList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
   <si>
     <t>Chores To Do</t>
   </si>
@@ -26,121 +26,121 @@
     <t/>
   </si>
   <si>
+    <t>clean boys bathroom pickup towels</t>
+  </si>
+  <si>
+    <t>take out trash</t>
+  </si>
+  <si>
+    <t>Hazel</t>
+  </si>
+  <si>
+    <t>sweep &amp; mop under bar stools &amp; area between sofa &amp; bar</t>
+  </si>
+  <si>
+    <t>sweep &amp; leaf blow back porch on both sides of gate</t>
+  </si>
+  <si>
+    <t>dust in the entry way and dinning room including desk area</t>
+  </si>
+  <si>
+    <t>empty trash can next to desk</t>
+  </si>
+  <si>
+    <t>dust fireplace &amp; mantel</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>clean &amp; wipe down stove &amp; counters by stove</t>
+  </si>
+  <si>
+    <t>clean &amp; wipe down counters in pantry</t>
+  </si>
+  <si>
+    <t>clean kitchen garbage cans area</t>
+  </si>
+  <si>
+    <t>Sift cat litter box in Daddy &amp; Renee's Room &amp; add new litter if needed, shake out &amp; clean mat and vacuum in front of litter box</t>
+  </si>
+  <si>
+    <t>DO NOT EMPTY OUT OLD LITTER</t>
+  </si>
+  <si>
     <t>sweep or vacuum living room &amp; mop</t>
   </si>
   <si>
     <t>move Daisy's crate &amp; sofas</t>
   </si>
   <si>
-    <t>Hazel</t>
+    <t>Ray</t>
   </si>
   <si>
     <t>clean, sweep &amp; mop kitchen bathroom</t>
   </si>
   <si>
-    <t>take out trash</t>
-  </si>
-  <si>
-    <t>dust in the entry way and dinning room including desk area</t>
-  </si>
-  <si>
-    <t>empty trash can next to desk</t>
+    <t>wipe off bar</t>
+  </si>
+  <si>
+    <t>pick up living room</t>
+  </si>
+  <si>
+    <t>fold &amp; put away blankets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty cat litter box in dinning room and add new litter shake out mat and sweep in front of litter box </t>
+  </si>
+  <si>
+    <t>dust around living room desk area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sweep &amp; leaf blow front porch </t>
+  </si>
+  <si>
+    <t>sweep or vacuum &amp; mop kitchen</t>
+  </si>
+  <si>
+    <t>including hall and area outside Daddy &amp; Renee's door, under counters &amp; in corners</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>sweep or vacuum &amp; mop kids bathroom</t>
+  </si>
+  <si>
+    <t>wipe down counters &amp; island in kitchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sweep or vacuum &amp; mop area by garage door </t>
   </si>
   <si>
     <t>pick up area by garage door &amp; vacuum out drawer</t>
   </si>
   <si>
-    <t xml:space="preserve">empty cat litter box in dinning room and add new litter shake out mat and sweep in front of litter box </t>
-  </si>
-  <si>
-    <t>clean boys bathroom pickup towels</t>
-  </si>
-  <si>
-    <t>Jesse</t>
-  </si>
-  <si>
-    <t>wipe down counters &amp; island in kitchen</t>
-  </si>
-  <si>
-    <t>clean kitchen garbage cans area</t>
+    <t>clean, dust &amp; straighten area on top of &amp; around Daisy's crate &amp; console bench under window</t>
+  </si>
+  <si>
+    <t>sweep or vacuum front of house &amp; mop</t>
+  </si>
+  <si>
+    <t>(entryway, dinning room, bedroom hall, hall leading to kitchen)</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>dust windows and doors</t>
   </si>
   <si>
     <t>empty/add new litter in cat litter box in storage closet, shake out mat under storage closet cat litter box &amp; sweep and mop storage closet</t>
   </si>
   <si>
-    <t>dust windows and doors</t>
-  </si>
-  <si>
-    <t>Sift cat litter box in Daddy &amp; Renee's Room &amp; add new litter if needed, shake out &amp; clean mat and vacuum in front of litter box</t>
-  </si>
-  <si>
-    <t>DO NOT EMPTY OUT OLD LITTER</t>
-  </si>
-  <si>
-    <t>sweep or vacuum front of house &amp; mop</t>
-  </si>
-  <si>
-    <t>(entryway, dinning room, bedroom hall, hall leading to kitchen)</t>
-  </si>
-  <si>
-    <t>Ray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sweep or vacuum &amp; mop area by garage door </t>
-  </si>
-  <si>
     <t>clean microwave with spray cleaner &amp; clorox wipes</t>
   </si>
   <si>
     <t>sweep or vacuum &amp; mop pantry</t>
-  </si>
-  <si>
-    <t>dust around living room desk area</t>
-  </si>
-  <si>
-    <t>sweep or vacuum &amp; mop kids bathroom</t>
-  </si>
-  <si>
-    <t>Ruby</t>
-  </si>
-  <si>
-    <t>clean &amp; wipe down stove &amp; counters by stove</t>
-  </si>
-  <si>
-    <t>sweep &amp; mop under bar stools &amp; area between sofa &amp; bar</t>
-  </si>
-  <si>
-    <t>pick up living room</t>
-  </si>
-  <si>
-    <t>fold &amp; put away blankets</t>
-  </si>
-  <si>
-    <t>clean, dust &amp; straighten area on top of &amp; around Daisy's crate &amp; console bench under window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sweep &amp; leaf blow front porch </t>
-  </si>
-  <si>
-    <t>sweep &amp; leaf blow back porch on both sides of gate</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>sweep or vacuum &amp; mop kitchen</t>
-  </si>
-  <si>
-    <t>including hall and area outside Daddy &amp; Renee's door, under counters &amp; in corners</t>
-  </si>
-  <si>
-    <t>clean &amp; wipe down counters in pantry</t>
-  </si>
-  <si>
-    <t>wipe off bar</t>
-  </si>
-  <si>
-    <t>dust fireplace &amp; mantel</t>
   </si>
 </sst>
 </file>
@@ -234,7 +234,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -290,7 +290,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s" s="3">
         <v>6</v>
@@ -301,10 +301,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s" s="3">
         <v>6</v>
@@ -315,10 +315,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s" s="6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s" s="3">
         <v>6</v>
@@ -329,7 +329,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s" s="7">
         <v>3</v>
@@ -343,13 +343,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>3</v>
@@ -357,13 +357,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s" s="3">
         <v>3</v>
@@ -371,13 +371,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s" s="3">
         <v>3</v>
@@ -385,69 +385,69 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B11" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="3">
+      <c r="C12" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="B12" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="4">
+      <c r="B13" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="B13" t="s" s="7">
+      <c r="C13" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="C13" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s" s="4">
+      <c r="D13" t="s" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="2">
+      <c r="A14" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="B14" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s" s="2">
+      <c r="B14" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s" s="3">
         <v>3</v>
@@ -455,13 +455,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="3">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s" s="6">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s" s="3">
         <v>3</v>
@@ -469,57 +469,57 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="B17" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="4">
+      <c r="B18" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="B18" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s" s="4">
-        <v>23</v>
-      </c>
-      <c r="D18" t="s" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="2">
+      <c r="B19" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B19" t="s" s="5">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s" s="2">
+      <c r="B20" t="s" s="5">
         <v>29</v>
       </c>
-      <c r="D19" t="s" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="3">
+      <c r="C20" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="B20" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s" s="3">
+      <c r="D20" t="s" s="2">
         <v>3</v>
       </c>
     </row>
@@ -531,7 +531,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s" s="3">
         <v>3</v>
@@ -542,10 +542,10 @@
         <v>32</v>
       </c>
       <c r="B22" t="s" s="6">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s" s="3">
         <v>3</v>
@@ -553,69 +553,69 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="3">
         <v>34</v>
       </c>
-      <c r="B23" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="D23" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="4">
+      <c r="B24" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="B24" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="2">
+      <c r="B25" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s" s="4">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="B25" t="s" s="5">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s" s="2">
+      <c r="B26" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="D25" t="s" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="3">
+      <c r="C26" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="B26" t="s" s="6">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="D26" t="s" s="3">
+      <c r="D26" t="s" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C27" t="s" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s" s="3">
         <v>3</v>
@@ -623,29 +623,43 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="3">
         <v>41</v>
       </c>
-      <c r="B28" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="D28" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="4">
+      <c r="B29" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="B29" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D29" t="s" s="4">
+      <c r="B30" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s" s="4">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
had to regenerate lost files
had to regenerate lost files
</commit_message>
<xml_diff>
--- a/ChorelistGenerator_Output/ChoreList.xlsx
+++ b/ChorelistGenerator_Output/ChoreList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
   <si>
     <t>Chores To Do</t>
   </si>
@@ -26,121 +26,121 @@
     <t/>
   </si>
   <si>
+    <t>sweep or vacuum front of house &amp; mop</t>
+  </si>
+  <si>
+    <t>(entryway, dinning room, bedroom hall, hall leading to kitchen)</t>
+  </si>
+  <si>
+    <t>Hazel</t>
+  </si>
+  <si>
+    <t>empty/add new litter in cat litter box in storage closet, shake out mat under storage closet cat litter box &amp; sweep and mop storage closet</t>
+  </si>
+  <si>
+    <t>clean microwave with spray cleaner &amp; clorox wipes</t>
+  </si>
+  <si>
+    <t>Sift cat litter box in Daddy &amp; Renee's Room &amp; add new litter if needed, shake out &amp; clean mat and vacuum in front of litter box</t>
+  </si>
+  <si>
+    <t>DO NOT EMPTY OUT OLD LITTER</t>
+  </si>
+  <si>
+    <t>dust fireplace &amp; mantel</t>
+  </si>
+  <si>
     <t>clean boys bathroom pickup towels</t>
   </si>
   <si>
     <t>take out trash</t>
   </si>
   <si>
-    <t>Hazel</t>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>clean, sweep &amp; mop kitchen bathroom</t>
+  </si>
+  <si>
+    <t>clean &amp; wipe down counters in pantry</t>
+  </si>
+  <si>
+    <t>pick up living room</t>
+  </si>
+  <si>
+    <t>fold &amp; put away blankets</t>
+  </si>
+  <si>
+    <t>sweep or vacuum &amp; mop pantry</t>
+  </si>
+  <si>
+    <t>dust around and straighten living room desk area</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>sweep or vacuum &amp; mop kitchen</t>
+  </si>
+  <si>
+    <t>including hall and area outside Daddy &amp; Renee's door, under counters &amp; in corners</t>
   </si>
   <si>
     <t>sweep &amp; mop under bar stools &amp; area between sofa &amp; bar</t>
   </si>
   <si>
+    <t>wipe off bar</t>
+  </si>
+  <si>
+    <t>dust in the entry way and dinning room including desk area</t>
+  </si>
+  <si>
+    <t>empty trash can next to desk</t>
+  </si>
+  <si>
+    <t>pick up area by garage door &amp; vacuum out drawer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty cat litter box in dinning room and add new litter shake out mat and sweep in front of litter box </t>
+  </si>
+  <si>
+    <t>clean &amp; wipe down stove &amp; counters by stove</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>sweep or vacuum &amp; mop kids bathroom</t>
+  </si>
+  <si>
+    <t>wipe down counters &amp; island in kitchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sweep or vacuum &amp; mop area by garage door </t>
+  </si>
+  <si>
+    <t>clean, dust &amp; straighten area on top of &amp; around Daisy's crate &amp; console bench under window</t>
+  </si>
+  <si>
+    <t>sweep or vacuum living room &amp; mop</t>
+  </si>
+  <si>
+    <t>move Daisy's crate &amp; sofas</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
     <t>sweep &amp; leaf blow back porch on both sides of gate</t>
   </si>
   <si>
-    <t>dust in the entry way and dinning room including desk area</t>
-  </si>
-  <si>
-    <t>empty trash can next to desk</t>
-  </si>
-  <si>
-    <t>dust fireplace &amp; mantel</t>
-  </si>
-  <si>
-    <t>Jesse</t>
-  </si>
-  <si>
-    <t>clean &amp; wipe down stove &amp; counters by stove</t>
-  </si>
-  <si>
-    <t>clean &amp; wipe down counters in pantry</t>
+    <t>dust windows and doors</t>
   </si>
   <si>
     <t>clean kitchen garbage cans area</t>
   </si>
   <si>
-    <t>Sift cat litter box in Daddy &amp; Renee's Room &amp; add new litter if needed, shake out &amp; clean mat and vacuum in front of litter box</t>
-  </si>
-  <si>
-    <t>DO NOT EMPTY OUT OLD LITTER</t>
-  </si>
-  <si>
-    <t>sweep or vacuum living room &amp; mop</t>
-  </si>
-  <si>
-    <t>move Daisy's crate &amp; sofas</t>
-  </si>
-  <si>
-    <t>Ray</t>
-  </si>
-  <si>
-    <t>clean, sweep &amp; mop kitchen bathroom</t>
-  </si>
-  <si>
-    <t>wipe off bar</t>
-  </si>
-  <si>
-    <t>pick up living room</t>
-  </si>
-  <si>
-    <t>fold &amp; put away blankets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">empty cat litter box in dinning room and add new litter shake out mat and sweep in front of litter box </t>
-  </si>
-  <si>
-    <t>dust around living room desk area</t>
-  </si>
-  <si>
     <t xml:space="preserve">sweep &amp; leaf blow front porch </t>
-  </si>
-  <si>
-    <t>sweep or vacuum &amp; mop kitchen</t>
-  </si>
-  <si>
-    <t>including hall and area outside Daddy &amp; Renee's door, under counters &amp; in corners</t>
-  </si>
-  <si>
-    <t>Ruby</t>
-  </si>
-  <si>
-    <t>sweep or vacuum &amp; mop kids bathroom</t>
-  </si>
-  <si>
-    <t>wipe down counters &amp; island in kitchen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sweep or vacuum &amp; mop area by garage door </t>
-  </si>
-  <si>
-    <t>pick up area by garage door &amp; vacuum out drawer</t>
-  </si>
-  <si>
-    <t>clean, dust &amp; straighten area on top of &amp; around Daisy's crate &amp; console bench under window</t>
-  </si>
-  <si>
-    <t>sweep or vacuum front of house &amp; mop</t>
-  </si>
-  <si>
-    <t>(entryway, dinning room, bedroom hall, hall leading to kitchen)</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>dust windows and doors</t>
-  </si>
-  <si>
-    <t>empty/add new litter in cat litter box in storage closet, shake out mat under storage closet cat litter box &amp; sweep and mop storage closet</t>
-  </si>
-  <si>
-    <t>clean microwave with spray cleaner &amp; clorox wipes</t>
-  </si>
-  <si>
-    <t>sweep or vacuum &amp; mop pantry</t>
   </si>
 </sst>
 </file>
@@ -234,7 +234,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -343,13 +343,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>3</v>
@@ -357,13 +357,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="B9" t="s" s="6">
-        <v>3</v>
-      </c>
       <c r="C9" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s" s="3">
         <v>3</v>
@@ -371,13 +371,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s" s="3">
         <v>14</v>
-      </c>
-      <c r="B10" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s" s="3">
-        <v>12</v>
       </c>
       <c r="D10" t="s" s="3">
         <v>3</v>
@@ -385,13 +385,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s" s="6">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s" s="3">
         <v>3</v>
@@ -399,13 +399,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="4">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s" s="7">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s" s="4">
         <v>3</v>
@@ -413,13 +413,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s" s="2">
         <v>3</v>
@@ -427,13 +427,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="3">
         <v>21</v>
-      </c>
-      <c r="B14" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s" s="3">
-        <v>20</v>
       </c>
       <c r="D14" t="s" s="3">
         <v>3</v>
@@ -441,13 +441,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s" s="3">
         <v>3</v>
@@ -455,13 +455,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s" s="6">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s" s="3">
         <v>3</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s" s="6">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s" s="3">
         <v>3</v>
@@ -483,13 +483,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s" s="3">
         <v>3</v>
@@ -497,13 +497,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="7">
         <v>3</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s" s="4">
         <v>3</v>
@@ -511,13 +511,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s" s="2">
         <v>3</v>
@@ -525,13 +525,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s" s="3">
         <v>31</v>
-      </c>
-      <c r="B21" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s" s="3">
-        <v>30</v>
       </c>
       <c r="D21" t="s" s="3">
         <v>3</v>
@@ -539,13 +539,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s" s="3">
         <v>3</v>
@@ -553,63 +553,63 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s" s="6">
         <v>3</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="B24" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="D24" t="s" s="3">
+      <c r="A24" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="4">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s" s="4">
-        <v>30</v>
-      </c>
-      <c r="D25" t="s" s="4">
+      <c r="A25" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s" s="5">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s" s="2">
+      <c r="A26" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s" s="3">
         <v>38</v>
       </c>
-      <c r="D26" t="s" s="2">
+      <c r="D26" t="s" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s" s="6">
         <v>3</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s" s="6">
         <v>3</v>
@@ -636,30 +636,16 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="B29" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s" s="3">
+      <c r="A29" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s" s="4">
         <v>38</v>
       </c>
-      <c r="D29" t="s" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="B30" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s" s="4">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s" s="4">
+      <c r="D29" t="s" s="4">
         <v>3</v>
       </c>
     </row>

</xml_diff>